<commit_message>
Inclusion du fichier de synthèse pour les résultats sur les flottants et léger ajustement de la légende des graphiques du fichier de synthèse pour les entiers
</commit_message>
<xml_diff>
--- a/Resultats/Entiers - Résultats.xlsx
+++ b/Resultats/Entiers - Résultats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederick the Great\Documents\GitHub\DockerCpuOverheadTesting\Resultats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AAF6A7-F441-4975-9F5C-668595CA4D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E04476-F85D-456E-97D8-735D95AC7972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,18 +457,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1582,12 +1571,26 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.76730714143760748"/>
+          <c:y val="0.12717945255846688"/>
+          <c:w val="0.22224899433262749"/>
+          <c:h val="0.1944697610655412"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -2289,12 +2292,26 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.86563452655489304"/>
+          <c:y val="0.12412371134020618"/>
+          <c:w val="0.12029335383209025"/>
+          <c:h val="7.7320128798333207E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -3792,7 +3809,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4453,7 +4470,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E23" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4474,7 +4491,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>
       <c r="B2" s="14" t="s">
         <v>15</v>
@@ -4483,7 +4500,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19"/>
       <c r="B3" s="14" t="s">
         <v>17</v>
@@ -4512,7 +4529,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
         <v>15</v>
@@ -4521,7 +4538,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
       <c r="B7" s="14" t="s">
         <v>24</v>
@@ -4539,7 +4556,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="14" t="s">
         <v>28</v>
@@ -4548,7 +4565,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="B10" s="14" t="s">
         <v>30</v>
@@ -4557,7 +4574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" s="14" t="s">
         <v>31</v>
@@ -4566,7 +4583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="14" t="s">
         <v>32</v>
@@ -4575,7 +4592,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="14" t="s">
         <v>34</v>
@@ -4584,7 +4601,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="B14" s="15" t="s">
         <v>36</v>
@@ -4604,7 +4621,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
       <c r="B16" s="14" t="s">
         <v>15</v>
@@ -4613,7 +4630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="14" t="s">
         <v>40</v>
@@ -4622,7 +4639,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
       <c r="B18" s="14" t="s">
         <v>26</v>
@@ -4640,7 +4657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="14" t="s">
         <v>45</v>
@@ -4649,7 +4666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="14" t="s">
         <v>46</v>
@@ -4658,7 +4675,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="15" t="s">
         <v>48</v>
@@ -4678,7 +4695,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="14" t="s">
         <v>15</v>
@@ -4687,7 +4704,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="14" t="s">
         <v>40</v>
@@ -4696,7 +4713,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="14" t="s">
         <v>52</v>
@@ -4705,7 +4722,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="14" t="s">
         <v>54</v>
@@ -4714,7 +4731,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="14" t="s">
         <v>56</v>
@@ -4723,7 +4740,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="14" t="s">
         <v>58</v>
@@ -4732,7 +4749,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="14" t="s">
         <v>60</v>
@@ -6139,7 +6156,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{263FB86D-35E9-4665-BD76-C9655B1CD1C7}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D53633E4-B3A2-4836-8621-294DFDF88276}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -6150,8 +6167,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (Natif)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (Natif)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{671BC30B-64D0-4A0F-9895-0D2CA0CBDCA2}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (Natif)'!D2:D51</xm:f>
+              <xm:sqref>D55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D6051AD8-E20E-4C7E-83A6-FB1D6D67759B}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (Natif)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0AC99F70-1986-4530-85CD-87DAB941F78A}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (Natif)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -6171,7 +6236,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0AC99F70-1986-4530-85CD-87DAB941F78A}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{263FB86D-35E9-4665-BD76-C9655B1CD1C7}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -6182,56 +6247,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (Natif)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D6051AD8-E20E-4C7E-83A6-FB1D6D67759B}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (Natif)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{671BC30B-64D0-4A0F-9895-0D2CA0CBDCA2}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (Natif)'!D2:D51</xm:f>
-              <xm:sqref>D55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D53633E4-B3A2-4836-8621-294DFDF88276}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (Natif)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (Natif)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -7625,7 +7642,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{26BC4944-7654-4BFA-9F72-24B1C359120F}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0FA95288-A489-4585-94C4-768758F6474C}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -7636,8 +7653,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (WSL2)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{4248C55C-E6A0-488D-9E03-C6F366FFF486}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2)'!D2:D51</xm:f>
+              <xm:sqref>D55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{BBA6465A-E308-4DD6-9A70-F5CB35F82A61}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0FA84A2C-672E-44AC-ACAA-ED61E0BF21BE}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -7657,7 +7722,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0FA84A2C-672E-44AC-ACAA-ED61E0BF21BE}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{26BC4944-7654-4BFA-9F72-24B1C359120F}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -7668,56 +7733,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{BBA6465A-E308-4DD6-9A70-F5CB35F82A61}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{4248C55C-E6A0-488D-9E03-C6F366FFF486}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!D2:D51</xm:f>
-              <xm:sqref>D55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0FA95288-A489-4585-94C4-768758F6474C}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (WSL2)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -9110,7 +9127,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{CFB2627E-8967-4A81-83E6-676B520A3425}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DFB037B2-CCDD-4B71-9593-4095BEADE567}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -9121,8 +9138,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (WSL2 - Processus)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{21B542ED-F386-45BD-8EF8-BEBA77635647}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2 - Processus)'!D2:D51</xm:f>
+              <xm:sqref>D55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{98184E74-9215-4257-A184-37176536AAA8}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2 - Processus)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{6B49AE29-6C9E-480F-8A0D-77BC2859D87C}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2 - Processus)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -9142,7 +9207,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{6B49AE29-6C9E-480F-8A0D-77BC2859D87C}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{CFB2627E-8967-4A81-83E6-676B520A3425}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -9153,56 +9218,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{98184E74-9215-4257-A184-37176536AAA8}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{21B542ED-F386-45BD-8EF8-BEBA77635647}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!D2:D51</xm:f>
-              <xm:sqref>D55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DFB037B2-CCDD-4B71-9593-4095BEADE567}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (WSL2 - Processus)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -10595,7 +10612,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5DC8D8CB-A05A-4FE8-BCF8-8A2476066B3F}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{CB50B3B6-4016-48CB-8198-CE38282339F8}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -10606,8 +10623,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (HyperV)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{A06034E8-42C7-472A-B067-EE811F57A0B4}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV)'!D2:D51</xm:f>
+              <xm:sqref>D55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DDFF044F-6546-4CF0-963C-9764D1216A74}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{948B6A77-9CAD-4F96-B620-E4761B6E212C}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -10627,7 +10692,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{948B6A77-9CAD-4F96-B620-E4761B6E212C}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5DC8D8CB-A05A-4FE8-BCF8-8A2476066B3F}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -10638,56 +10703,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DDFF044F-6546-4CF0-963C-9764D1216A74}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{A06034E8-42C7-472A-B067-EE811F57A0B4}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!D2:D51</xm:f>
-              <xm:sqref>D55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{CB50B3B6-4016-48CB-8198-CE38282339F8}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (HyperV)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -12080,7 +12097,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0B58E305-8FE4-447D-AD29-B0D933ADB202}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{3B759F57-5925-482A-9086-0B51A14E2420}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -12091,8 +12108,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (HyperV - Processus)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{1EA3185D-40DD-47E9-A39C-1367329AB1A7}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV - Processus)'!D2:D51</xm:f>
+              <xm:sqref>D55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B4EACD82-77AA-48D9-A91E-A39ABF91BBAB}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV - Processus)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{48A1F807-54EC-4B10-844B-207851B03EB3}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV - Processus)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -12112,7 +12177,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{48A1F807-54EC-4B10-844B-207851B03EB3}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0B58E305-8FE4-447D-AD29-B0D933ADB202}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -12123,56 +12188,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B4EACD82-77AA-48D9-A91E-A39ABF91BBAB}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{1EA3185D-40DD-47E9-A39C-1367329AB1A7}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!D2:D51</xm:f>
-              <xm:sqref>D55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{3B759F57-5925-482A-9086-0B51A14E2420}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (HyperV - Processus)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -13565,7 +13582,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{C422E0C4-9C93-4E2A-A077-186C8471DC37}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{05DF6556-8BB2-4C26-BA82-557146EF9EEF}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -13576,8 +13593,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Linux (Natif)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Linux (Natif)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{AFDF9753-5CE6-40F4-A926-3D0D6A435DD2}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Natif)'!D2:D51</xm:f>
+              <xm:sqref>D55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{1FA50543-1619-4C76-BA32-FA54FFF9EEF0}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Natif)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5411D816-8D3B-4A0E-A036-09C6F257009C}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Natif)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -13597,7 +13662,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5411D816-8D3B-4A0E-A036-09C6F257009C}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{C422E0C4-9C93-4E2A-A077-186C8471DC37}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -13608,56 +13673,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Linux (Natif)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{1FA50543-1619-4C76-BA32-FA54FFF9EEF0}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Natif)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{AFDF9753-5CE6-40F4-A926-3D0D6A435DD2}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Natif)'!D2:D51</xm:f>
-              <xm:sqref>D55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{05DF6556-8BB2-4C26-BA82-557146EF9EEF}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Natif)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Linux (Natif)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -15050,7 +15067,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{7AF38403-7A79-4F1E-8FAD-23629879CF02}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{8A9F5D4B-DC6F-47C4-90FC-816734A33D56}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -15061,8 +15078,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Linux (Docker)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Linux (Docker)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{6BED89EE-1C79-4E16-BC11-017F1B50BD3F}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Docker)'!D2:D51</xm:f>
+              <xm:sqref>D55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DCCDEE7B-7404-4AB4-BFE7-57E07920CD05}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Docker)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B0D1C296-46A8-49F3-BBE8-C4AF5BB63750}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Docker)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -15082,7 +15147,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B0D1C296-46A8-49F3-BBE8-C4AF5BB63750}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{7AF38403-7A79-4F1E-8FAD-23629879CF02}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -15093,56 +15158,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Linux (Docker)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DCCDEE7B-7404-4AB4-BFE7-57E07920CD05}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Docker)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{6BED89EE-1C79-4E16-BC11-017F1B50BD3F}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Docker)'!D2:D51</xm:f>
-              <xm:sqref>D55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{8A9F5D4B-DC6F-47C4-90FC-816734A33D56}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Docker)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Linux (Docker)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
Mise à jour des fichiers de synthèse des résultats obtenus pour les trois tests
</commit_message>
<xml_diff>
--- a/Resultats/Entiers - Résultats.xlsx
+++ b/Resultats/Entiers - Résultats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederick the Great\Documents\GitHub\DockerCpuOverheadTesting\Resultats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E04476-F85D-456E-97D8-735D95AC7972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F357B1-9B9E-43BD-B6AB-1770142F9E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>entierLimite</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Disque dur</t>
+  </si>
+  <si>
+    <t>Écart-type (% de moyenne)</t>
   </si>
 </sst>
 </file>
@@ -580,7 +583,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Résultats!$C$3,Résultats!$F$3,Résultats!$I$3,Résultats!$L$3,Résultats!$O$3,Résultats!$R$3)</c:f>
+                <c:f>(Résultats!$D$3,Résultats!$H$3,Résultats!$L$3,Résultats!$P$3,Résultats!$T$3,Résultats!$X$3)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -607,7 +610,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Résultats!$C$3,Résultats!$F$3,Résultats!$I$3,Résultats!$L$3,Résultats!$O$3,Résultats!$R$3)</c:f>
+                <c:f>(Résultats!$D$3,Résultats!$H$3,Résultats!$L$3,Résultats!$P$3,Résultats!$T$3,Résultats!$X$3)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -648,7 +651,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>(Résultats!$D$1,Résultats!$G$1,Résultats!$J$1,Résultats!$M$1,Résultats!$P$1,Résultats!$S$1)</c:f>
+              <c:f>(Résultats!$E$1,Résultats!$I$1,Résultats!$M$1,Résultats!$Q$1,Résultats!$U$1,Résultats!$Y$1)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -675,7 +678,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Résultats!$D$3,Résultats!$G$3,Résultats!$J$3,Résultats!$M$3,Résultats!$P$3,Résultats!$S$3)</c:f>
+              <c:f>(Résultats!$E$3,Résultats!$I$3,Résultats!$M$3,Résultats!$Q$3,Résultats!$U$3,Résultats!$Y$3)</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="6"/>
@@ -736,54 +739,54 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Résultats!$C$4,Résultats!$F$4,Résultats!$I$4,Résultats!$L$4,Résultats!$O$4,Résultats!$R$4)</c:f>
+                <c:f>(Résultats!$D$4,Résultats!$H$4,Résultats!$L$4,Résultats!$P$4,Résultats!$T$4,Résultats!$X$4)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>3.8143838451164806E-2</c:v>
+                    <c:v>3.9572822211740792E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.1139017620676176E-2</c:v>
+                    <c:v>1.1287707531793371E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.6750279292270469E-3</c:v>
+                    <c:v>6.7612927647956117E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.8157876531060786E-2</c:v>
+                    <c:v>1.8405104172967486E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>9.3186751015148141E-3</c:v>
+                    <c:v>9.4687838218795971E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3.8716754111385939E-3</c:v>
+                    <c:v>3.9518520206414049E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Résultats!$C$4,Résultats!$F$4,Résultats!$I$4,Résultats!$L$4,Résultats!$O$4,Résultats!$R$4)</c:f>
+                <c:f>(Résultats!$D$4,Résultats!$H$4,Résultats!$L$4,Résultats!$P$4,Résultats!$T$4,Résultats!$X$4)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>3.8143838451164806E-2</c:v>
+                    <c:v>3.9572822211740792E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.1139017620676176E-2</c:v>
+                    <c:v>1.1287707531793371E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.6750279292270469E-3</c:v>
+                    <c:v>6.7612927647956117E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.8157876531060786E-2</c:v>
+                    <c:v>1.8405104172967486E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>9.3186751015148141E-3</c:v>
+                    <c:v>9.4687838218795971E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3.8716754111385939E-3</c:v>
+                    <c:v>3.9518520206414049E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -804,7 +807,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>(Résultats!$D$1,Résultats!$G$1,Résultats!$J$1,Résultats!$M$1,Résultats!$P$1,Résultats!$S$1)</c:f>
+              <c:f>(Résultats!$E$1,Résultats!$I$1,Résultats!$M$1,Résultats!$Q$1,Résultats!$U$1,Résultats!$Y$1)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -831,7 +834,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Résultats!$D$4,Résultats!$G$4,Résultats!$J$4,Résultats!$M$4,Résultats!$P$4,Résultats!$S$4)</c:f>
+              <c:f>(Résultats!$E$4,Résultats!$I$4,Résultats!$M$4,Résultats!$Q$4,Résultats!$U$4,Résultats!$Y$4)</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="6"/>
@@ -892,54 +895,54 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Résultats!$C$5,Résultats!$F$5,Résultats!$I$5,Résultats!$L$5,Résultats!$O$5,Résultats!$R$5)</c:f>
+                <c:f>(Résultats!$D$5,Résultats!$H$5,Résultats!$L$5,Résultats!$P$5,Résultats!$T$5,Résultats!$X$5)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>3.2446931109419638E-2</c:v>
+                    <c:v>3.237229143877688E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.9598648734462464E-3</c:v>
+                    <c:v>7.9790095186833294E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.5752549250406803E-3</c:v>
+                    <c:v>6.5825868747783943E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.6874493700676389E-2</c:v>
+                    <c:v>1.6940770444977552E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.0673429285274293E-3</c:v>
+                    <c:v>7.1010165772533961E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.6198695226596607E-3</c:v>
+                    <c:v>4.6392807727951768E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Résultats!$C$5,Résultats!$F$5,Résultats!$I$5,Résultats!$L$5,Résultats!$O$5,Résultats!$R$5)</c:f>
+                <c:f>(Résultats!$D$5,Résultats!$H$5,Résultats!$L$5,Résultats!$P$5,Résultats!$T$5,Résultats!$X$5)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>3.2446931109419638E-2</c:v>
+                    <c:v>3.237229143877688E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.9598648734462464E-3</c:v>
+                    <c:v>7.9790095186833294E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.5752549250406803E-3</c:v>
+                    <c:v>6.5825868747783943E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.6874493700676389E-2</c:v>
+                    <c:v>1.6940770444977552E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.0673429285274293E-3</c:v>
+                    <c:v>7.1010165772533961E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.6198695226596607E-3</c:v>
+                    <c:v>4.6392807727951768E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -960,7 +963,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>(Résultats!$D$1,Résultats!$G$1,Résultats!$J$1,Résultats!$M$1,Résultats!$P$1,Résultats!$S$1)</c:f>
+              <c:f>(Résultats!$E$1,Résultats!$I$1,Résultats!$M$1,Résultats!$Q$1,Résultats!$U$1,Résultats!$Y$1)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -987,7 +990,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Résultats!$D$5,Résultats!$G$5,Résultats!$J$5,Résultats!$M$5,Résultats!$P$5,Résultats!$S$5)</c:f>
+              <c:f>(Résultats!$E$5,Résultats!$I$5,Résultats!$M$5,Résultats!$Q$5,Résultats!$U$5,Résultats!$Y$5)</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1048,54 +1051,54 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Résultats!$C$6,Résultats!$F$6,Résultats!$I$6,Résultats!$L$6,Résultats!$O$6,Résultats!$R$6)</c:f>
+                <c:f>(Résultats!$D$6,Résultats!$H$6,Résultats!$L$6,Résultats!$P$6,Résultats!$T$6,Résultats!$X$6)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>3.6543665828993981E-2</c:v>
+                    <c:v>3.764850225892085E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7535340799326442E-2</c:v>
+                    <c:v>1.7905427061160578E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.1190091655060194E-3</c:v>
+                    <c:v>7.2468358347251138E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.8325200265252344E-2</c:v>
+                    <c:v>1.8662019520956093E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.7723554060881882E-3</c:v>
+                    <c:v>8.9686725494884257E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.051776773270825E-3</c:v>
+                    <c:v>4.1654061719799528E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Résultats!$C$6,Résultats!$F$6,Résultats!$I$6,Résultats!$L$6,Résultats!$O$6,Résultats!$R$6)</c:f>
+                <c:f>(Résultats!$D$6,Résultats!$H$6,Résultats!$L$6,Résultats!$P$6,Résultats!$T$6,Résultats!$X$6)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>3.6543665828993981E-2</c:v>
+                    <c:v>3.764850225892085E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.7535340799326442E-2</c:v>
+                    <c:v>1.7905427061160578E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.1190091655060194E-3</c:v>
+                    <c:v>7.2468358347251138E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.8325200265252344E-2</c:v>
+                    <c:v>1.8662019520956093E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.7723554060881882E-3</c:v>
+                    <c:v>8.9686725494884257E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>4.051776773270825E-3</c:v>
+                    <c:v>4.1654061719799528E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1116,7 +1119,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>(Résultats!$D$1,Résultats!$G$1,Résultats!$J$1,Résultats!$M$1,Résultats!$P$1,Résultats!$S$1)</c:f>
+              <c:f>(Résultats!$E$1,Résultats!$I$1,Résultats!$M$1,Résultats!$Q$1,Résultats!$U$1,Résultats!$Y$1)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1143,7 +1146,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Résultats!$D$6,Résultats!$G$6,Résultats!$J$6,Résultats!$M$6,Résultats!$P$6,Résultats!$S$6)</c:f>
+              <c:f>(Résultats!$E$6,Résultats!$I$6,Résultats!$M$6,Résultats!$Q$6,Résultats!$U$6,Résultats!$Y$6)</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1204,54 +1207,54 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Résultats!$C$7,Résultats!$F$7,Résultats!$I$7,Résultats!$L$7,Résultats!$O$7,Résultats!$R$7)</c:f>
+                <c:f>(Résultats!$D$7,Résultats!$H$7,Résultats!$L$7,Résultats!$P$7,Résultats!$T$7,Résultats!$X$7)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>4.0422386904714627E-2</c:v>
+                    <c:v>4.0515373006697213E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.9338702582066305E-3</c:v>
+                    <c:v>7.947227745262719E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.9401327983209552E-3</c:v>
+                    <c:v>5.9355471346882278E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.6336363900456657E-2</c:v>
+                    <c:v>1.6408699176936003E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.0208104174399217E-3</c:v>
+                    <c:v>4.0474350170677893E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3.7398917875664985E-3</c:v>
+                    <c:v>3.7643622233670565E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Résultats!$C$7,Résultats!$F$7,Résultats!$I$7,Résultats!$L$7,Résultats!$O$7,Résultats!$R$7)</c:f>
+                <c:f>(Résultats!$D$7,Résultats!$H$7,Résultats!$L$7,Résultats!$P$7,Résultats!$T$7,Résultats!$X$7)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>4.0422386904714627E-2</c:v>
+                    <c:v>4.0515373006697213E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.9338702582066305E-3</c:v>
+                    <c:v>7.947227745262719E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.9401327983209552E-3</c:v>
+                    <c:v>5.9355471346882278E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.6336363900456657E-2</c:v>
+                    <c:v>1.6408699176936003E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.0208104174399217E-3</c:v>
+                    <c:v>4.0474350170677893E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3.7398917875664985E-3</c:v>
+                    <c:v>3.7643622233670565E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1272,7 +1275,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>(Résultats!$D$1,Résultats!$G$1,Résultats!$J$1,Résultats!$M$1,Résultats!$P$1,Résultats!$S$1)</c:f>
+              <c:f>(Résultats!$E$1,Résultats!$I$1,Résultats!$M$1,Résultats!$Q$1,Résultats!$U$1,Résultats!$Y$1)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1299,7 +1302,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Résultats!$D$7,Résultats!$G$7,Résultats!$J$7,Résultats!$M$7,Résultats!$P$7,Résultats!$S$7)</c:f>
+              <c:f>(Résultats!$E$7,Résultats!$I$7,Résultats!$M$7,Résultats!$Q$7,Résultats!$U$7,Résultats!$Y$7)</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1493,7 +1496,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>Charge computationnelle</a:t>
+                  <a:t>Surcharge computationnelle</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1770,7 +1773,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Résultats!$C$8,Résultats!$F$8,Résultats!$I$8,Résultats!$L$8,Résultats!$O$8,Résultats!$R$8)</c:f>
+                <c:f>(Résultats!$D$8,Résultats!$H$8,Résultats!$L$8,Résultats!$P$8,Résultats!$T$8,Résultats!$X$8)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -1797,7 +1800,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Résultats!$C$8,Résultats!$F$8,Résultats!$I$8,Résultats!$L$8,Résultats!$O$8,Résultats!$R$8)</c:f>
+                <c:f>(Résultats!$D$8,Résultats!$H$8,Résultats!$L$8,Résultats!$P$8,Résultats!$T$8,Résultats!$X$8)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -1838,7 +1841,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>(Résultats!$D$1,Résultats!$G$1,Résultats!$J$1,Résultats!$M$1,Résultats!$P$1,Résultats!$S$1)</c:f>
+              <c:f>(Résultats!$E$1,Résultats!$I$1,Résultats!$M$1,Résultats!$Q$1,Résultats!$U$1,Résultats!$Y$1)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1865,7 +1868,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Résultats!$D$8,Résultats!$G$8,Résultats!$J$8,Résultats!$M$8,Résultats!$P$8,Résultats!$S$8)</c:f>
+              <c:f>(Résultats!$E$8,Résultats!$I$8,Résultats!$M$8,Résultats!$Q$8,Résultats!$U$8,Résultats!$Y$8)</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1926,54 +1929,54 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Résultats!$C$9,Résultats!$F$9,Résultats!$I$9,Résultats!$L$9,Résultats!$O$9,Résultats!$R$9)</c:f>
+                <c:f>(Résultats!$D$9,Résultats!$H$9,Résultats!$L$9,Résultats!$P$9,Résultats!$T$9,Résultats!$X$9)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>5.1954349534846435E-2</c:v>
+                    <c:v>5.387185018583026E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.9194035510486093E-2</c:v>
+                    <c:v>1.9862609811936872E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.1367129336496614E-2</c:v>
+                    <c:v>1.1847762235028921E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.5961084712791708E-2</c:v>
+                    <c:v>1.6784590322652424E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.937819187904714E-3</c:v>
+                    <c:v>9.4488602947616664E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3.5648143489678498E-3</c:v>
+                    <c:v>3.8375607826333737E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Résultats!$C$9,Résultats!$F$9,Résultats!$I$9,Résultats!$L$9,Résultats!$O$9,Résultats!$R$9)</c:f>
+                <c:f>(Résultats!$D$9,Résultats!$H$9,Résultats!$L$9,Résultats!$P$9,Résultats!$T$9,Résultats!$X$9)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>5.1954349534846435E-2</c:v>
+                    <c:v>5.387185018583026E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.9194035510486093E-2</c:v>
+                    <c:v>1.9862609811936872E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.1367129336496614E-2</c:v>
+                    <c:v>1.1847762235028921E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.5961084712791708E-2</c:v>
+                    <c:v>1.6784590322652424E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.937819187904714E-3</c:v>
+                    <c:v>9.4488602947616664E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>3.5648143489678498E-3</c:v>
+                    <c:v>3.8375607826333737E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1994,7 +1997,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>(Résultats!$D$1,Résultats!$G$1,Résultats!$J$1,Résultats!$M$1,Résultats!$P$1,Résultats!$S$1)</c:f>
+              <c:f>(Résultats!$E$1,Résultats!$I$1,Résultats!$M$1,Résultats!$Q$1,Résultats!$U$1,Résultats!$Y$1)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2021,7 +2024,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Résultats!$D$9,Résultats!$G$9,Résultats!$J$9,Résultats!$M$9,Résultats!$P$9,Résultats!$S$9)</c:f>
+              <c:f>(Résultats!$E$9,Résultats!$I$9,Résultats!$M$9,Résultats!$Q$9,Résultats!$U$9,Résultats!$Y$9)</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2214,7 +2217,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>Charge computationnelle</a:t>
+                  <a:t>Surcharge computationnelle</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2282,6 +2285,7 @@
         <c:crossAx val="1666678192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2297,12 +2301,607 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86563452655489304"/>
-          <c:y val="0.12412371134020618"/>
+          <c:x val="0.86563453703117177"/>
+          <c:y val="8.9759450171821312E-2"/>
           <c:w val="0.12029335383209025"/>
           <c:h val="7.7320128798333207E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Résultats moyens du test pour les entiers dans les environnement natifs Linux et Windows</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Résultats!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Windows (Natif)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Résultats!$E$1,Résultats!$I$1,Résultats!$M$1,Résultats!$Q$1,Résultats!$U$1,Résultats!$Y$1)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500000000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Résultats!$B$3,Résultats!$F$3,Résultats!$J$3,Résultats!$N$3,Résultats!$R$3,Résultats!$V$3)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.0859999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33262000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.038059999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4328800000000008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.143359999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E4DF-47AE-9D0F-C9092973AA04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Résultats!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linux (Natif)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Résultats!$E$1,Résultats!$I$1,Résultats!$M$1,Résultats!$Q$1,Résultats!$U$1,Résultats!$Y$1)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000000000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000000000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500000000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Résultats!$B$8,Résultats!$F$8,Résultats!$J$8,Résultats!$N$8,Résultats!$R$8,Résultats!$V$8)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.2859999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33532000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70478000000000018</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0511999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4575399999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.305420000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E4DF-47AE-9D0F-C9092973AA04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="361279920"/>
+        <c:axId val="361274928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="361279920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Limite supérieure (entierLimite) du programme primesieve</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="361274928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="361274928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Temps</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> de calcul (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="361279920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:solidFill>
@@ -2421,6 +3020,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3466,6 +4105,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3476,7 +4618,7 @@
       <xdr:rowOff>195261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -3506,16 +4648,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>149679</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>17689</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3535,6 +4677,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>84364</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>13606</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>136072</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DBD4F46-C946-411B-A6B6-AB84055664DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3806,65 +4984,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE14D12C-CC7C-4B19-84E4-3D9A7ECB11D5}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9"/>
-      <c r="D1" s="9">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9">
         <v>1000000000</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9">
         <v>5000000000</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9">
-        <v>10000000000</v>
-      </c>
+      <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9">
+        <v>10000000000</v>
+      </c>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9">
         <v>50000000000</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9">
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9">
         <v>100000000000</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9">
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9">
         <v>500000000000</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3872,31 +5062,31 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>11</v>
@@ -3908,19 +5098,37 @@
         <v>2</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="V2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -3928,76 +5136,100 @@
         <f>'Windows (Natif)'!$B$52</f>
         <v>6.0859999999999997E-2</v>
       </c>
-      <c r="C3" s="10">
-        <f>'Windows (Natif)'!$B$54</f>
+      <c r="C3" s="5">
+        <f>'Windows (Natif)'!$B$53</f>
+        <v>2.000099997500125E-3</v>
+      </c>
+      <c r="D3" s="10">
+        <f>C3/$B$3</f>
         <v>3.2863950008217631E-2</v>
       </c>
-      <c r="D3" s="10">
+      <c r="E3" s="10">
         <f>B3/$B$3</f>
         <v>1</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F3" s="5">
         <f>'Windows (Natif)'!$D$52</f>
         <v>0.33262000000000003</v>
       </c>
-      <c r="F3" s="10">
-        <f>'Windows (Natif)'!$D$54</f>
+      <c r="G3" s="5">
+        <f>'Windows (Natif)'!$D$53</f>
+        <v>2.7047365860652698E-3</v>
+      </c>
+      <c r="H3" s="10">
+        <f>G3/$F$3</f>
         <v>8.1316114066059455E-3</v>
       </c>
-      <c r="G3" s="10">
-        <f>E3/$E$3</f>
+      <c r="I3" s="10">
+        <f>F3/$F$3</f>
         <v>1</v>
       </c>
-      <c r="H3" s="5">
+      <c r="J3" s="5">
         <f>'Windows (Natif)'!$F$52</f>
         <v>0.69950000000000001</v>
       </c>
-      <c r="I3" s="10">
-        <f>'Windows (Natif)'!$F$54</f>
+      <c r="K3" s="5">
+        <f>'Windows (Natif)'!$F$53</f>
+        <v>4.7423622805517545E-3</v>
+      </c>
+      <c r="L3" s="10">
+        <f>K3/$J$3</f>
         <v>6.7796458621183055E-3</v>
       </c>
-      <c r="J3" s="10">
-        <f>H3/$H$3</f>
+      <c r="M3" s="10">
+        <f>J3/$J$3</f>
         <v>1</v>
       </c>
-      <c r="K3" s="5">
+      <c r="N3" s="5">
         <f>'Windows (Natif)'!$H$52</f>
         <v>4.038059999999998</v>
       </c>
-      <c r="L3" s="10">
-        <f>'Windows (Natif)'!$H$54</f>
+      <c r="O3" s="5">
+        <f>'Windows (Natif)'!$H$53</f>
+        <v>7.5502691342759456E-2</v>
+      </c>
+      <c r="P3" s="10">
+        <f>O3/$N$3</f>
         <v>1.8697763614894156E-2</v>
       </c>
-      <c r="M3" s="10">
-        <f>K3/$K$3</f>
+      <c r="Q3" s="10">
+        <f>N3/$N$3</f>
         <v>1</v>
       </c>
-      <c r="N3" s="5">
+      <c r="R3" s="5">
         <f>'Windows (Natif)'!$J$52</f>
         <v>8.4328800000000008</v>
       </c>
-      <c r="O3" s="10">
-        <f>'Windows (Natif)'!$J$54</f>
+      <c r="S3" s="5">
+        <f>'Windows (Natif)'!$J$53</f>
+        <v>8.9353374866313839E-2</v>
+      </c>
+      <c r="T3" s="10">
+        <f>S3/$R$3</f>
         <v>1.0595831420145174E-2</v>
       </c>
-      <c r="P3" s="10">
-        <f>N3/$N$3</f>
+      <c r="U3" s="10">
+        <f>R3/$R$3</f>
         <v>1</v>
       </c>
-      <c r="Q3" s="5">
+      <c r="V3" s="5">
         <f>'Windows (Natif)'!$L$52</f>
         <v>46.143359999999994</v>
       </c>
-      <c r="R3" s="10">
-        <f>'Windows (Natif)'!$L$54</f>
+      <c r="W3" s="5">
+        <f>'Windows (Natif)'!$L$53</f>
+        <v>0.14247873665919392</v>
+      </c>
+      <c r="X3" s="10">
+        <f>W3/$V$3</f>
         <v>3.0877408289988837E-3</v>
       </c>
-      <c r="S3" s="10">
-        <f>Q3/$Q$3</f>
+      <c r="Y3" s="10">
+        <f>V3/$V$3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -4005,76 +5237,100 @@
         <f>'Windows (WSL2)'!$B$52</f>
         <v>6.3139999999999974E-2</v>
       </c>
-      <c r="C4" s="10">
-        <f>'Windows (WSL2)'!$B$54</f>
-        <v>3.8143838451164806E-2</v>
+      <c r="C4" s="5">
+        <f>'Windows (WSL2)'!$B$53</f>
+        <v>2.4084019598065447E-3</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" ref="D4:D7" si="0">B4/$B$3</f>
+        <f t="shared" ref="D4:D7" si="0">C4/$B$3</f>
+        <v>3.9572822211740792E-2</v>
+      </c>
+      <c r="E4" s="10">
+        <f>B4/$B$3</f>
         <v>1.037463029904699</v>
       </c>
-      <c r="E4" s="5">
+      <c r="F4" s="5">
         <f>'Windows (WSL2)'!$D$52</f>
         <v>0.33705999999999997</v>
       </c>
-      <c r="F4" s="10">
-        <f>'Windows (WSL2)'!$D$54</f>
-        <v>1.1139017620676176E-2</v>
-      </c>
-      <c r="G4" s="10">
-        <f t="shared" ref="G4:G7" si="1">E4/$E$3</f>
+      <c r="G4" s="5">
+        <f>'Windows (WSL2)'!$D$53</f>
+        <v>3.7545172792251115E-3</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" ref="H4:H7" si="1">G4/$F$3</f>
+        <v>1.1287707531793371E-2</v>
+      </c>
+      <c r="I4" s="10">
+        <f>F4/$F$3</f>
         <v>1.0133485659310923</v>
       </c>
-      <c r="H4" s="5">
+      <c r="J4" s="5">
         <f>'Windows (WSL2)'!$F$52</f>
         <v>0.70853999999999984</v>
       </c>
-      <c r="I4" s="10">
-        <f>'Windows (WSL2)'!$F$54</f>
-        <v>6.6750279292270469E-3</v>
-      </c>
-      <c r="J4" s="10">
-        <f t="shared" ref="J4:J7" si="2">H4/$H$3</f>
+      <c r="K4" s="5">
+        <f>'Windows (WSL2)'!$F$53</f>
+        <v>4.7295242889745306E-3</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" ref="L4:L7" si="2">K4/$J$3</f>
+        <v>6.7612927647956117E-3</v>
+      </c>
+      <c r="M4" s="10">
+        <f>J4/$J$3</f>
         <v>1.0129235167977124</v>
       </c>
-      <c r="K4" s="5">
+      <c r="N4" s="5">
         <f>'Windows (WSL2)'!$H$52</f>
         <v>4.0930400000000002</v>
       </c>
-      <c r="L4" s="10">
-        <f>'Windows (WSL2)'!$H$54</f>
-        <v>1.8157876531060786E-2</v>
-      </c>
-      <c r="M4" s="10">
-        <f t="shared" ref="M4:M7" si="3">K4/$K$3</f>
+      <c r="O4" s="5">
+        <f>'Windows (WSL2)'!$H$53</f>
+        <v>7.4320914956693046E-2</v>
+      </c>
+      <c r="P4" s="10">
+        <f t="shared" ref="P4:P7" si="3">O4/$N$3</f>
+        <v>1.8405104172967486E-2</v>
+      </c>
+      <c r="Q4" s="10">
+        <f>N4/$N$3</f>
         <v>1.0136154490027396</v>
       </c>
-      <c r="N4" s="5">
+      <c r="R4" s="5">
         <f>'Windows (WSL2)'!$J$52</f>
         <v>8.5687200000000008</v>
       </c>
-      <c r="O4" s="10">
-        <f>'Windows (WSL2)'!$J$54</f>
-        <v>9.3186751015148141E-3</v>
-      </c>
-      <c r="P4" s="10">
-        <f t="shared" ref="P4:P7" si="4">N4/$N$3</f>
+      <c r="S4" s="5">
+        <f>'Windows (WSL2)'!$J$53</f>
+        <v>7.9849117715852028E-2</v>
+      </c>
+      <c r="T4" s="10">
+        <f t="shared" ref="T4:T7" si="4">S4/$R$3</f>
+        <v>9.4687838218795971E-3</v>
+      </c>
+      <c r="U4" s="10">
+        <f>R4/$R$3</f>
         <v>1.0161083757862082</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="V4" s="5">
         <f>'Windows (WSL2)'!$L$52</f>
         <v>47.098920000000007</v>
       </c>
-      <c r="R4" s="10">
-        <f>'Windows (WSL2)'!$L$54</f>
-        <v>3.8716754111385939E-3</v>
-      </c>
-      <c r="S4" s="10">
-        <f t="shared" ref="S4:S7" si="5">Q4/$Q$3</f>
+      <c r="W4" s="5">
+        <f>'Windows (WSL2)'!$L$53</f>
+        <v>0.18235173045518377</v>
+      </c>
+      <c r="X4" s="10">
+        <f t="shared" ref="X4:X7" si="5">W4/$V$3</f>
+        <v>3.9518520206414049E-3</v>
+      </c>
+      <c r="Y4" s="10">
+        <f t="shared" ref="Y4:Y7" si="6">V4/$V$3</f>
         <v>1.0207085049723299</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -4082,76 +5338,100 @@
         <f>'Windows (WSL2 - Processus)'!$B$52</f>
         <v>6.0720000000000003E-2</v>
       </c>
-      <c r="C5" s="10">
-        <f>'Windows (WSL2 - Processus)'!$B$54</f>
-        <v>3.2446931109419638E-2</v>
+      <c r="C5" s="5">
+        <f>'Windows (WSL2 - Processus)'!$B$53</f>
+        <v>1.9701776569639607E-3</v>
       </c>
       <c r="D5" s="10">
         <f t="shared" si="0"/>
+        <v>3.237229143877688E-2</v>
+      </c>
+      <c r="E5" s="10">
+        <f>B5/$B$3</f>
         <v>0.99769963851462384</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <f>'Windows (WSL2 - Processus)'!$D$52</f>
         <v>0.33342000000000022</v>
       </c>
-      <c r="F5" s="10">
-        <f>'Windows (WSL2 - Processus)'!$D$54</f>
-        <v>7.9598648734462464E-3</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="G5" s="5">
+        <f>'Windows (WSL2 - Processus)'!$D$53</f>
+        <v>2.6539781461044493E-3</v>
+      </c>
+      <c r="H5" s="10">
         <f t="shared" si="1"/>
+        <v>7.9790095186833294E-3</v>
+      </c>
+      <c r="I5" s="10">
+        <f>F5/$F$3</f>
         <v>1.0024051470146118</v>
       </c>
-      <c r="H5" s="5">
+      <c r="J5" s="5">
         <f>'Windows (WSL2 - Processus)'!$F$52</f>
         <v>0.7002799999999999</v>
       </c>
-      <c r="I5" s="10">
-        <f>'Windows (WSL2 - Processus)'!$F$54</f>
-        <v>6.5752549250406803E-3</v>
-      </c>
-      <c r="J5" s="10">
+      <c r="K5" s="5">
+        <f>'Windows (WSL2 - Processus)'!$F$53</f>
+        <v>4.6045195189074869E-3</v>
+      </c>
+      <c r="L5" s="10">
         <f t="shared" si="2"/>
+        <v>6.5825868747783943E-3</v>
+      </c>
+      <c r="M5" s="10">
+        <f>J5/$J$3</f>
         <v>1.0011150822015724</v>
       </c>
-      <c r="K5" s="5">
+      <c r="N5" s="5">
         <f>'Windows (WSL2 - Processus)'!$H$52</f>
         <v>4.0539199999999989</v>
       </c>
-      <c r="L5" s="10">
-        <f>'Windows (WSL2 - Processus)'!$H$54</f>
-        <v>1.6874493700676389E-2</v>
-      </c>
-      <c r="M5" s="10">
+      <c r="O5" s="5">
+        <f>'Windows (WSL2 - Processus)'!$H$53</f>
+        <v>6.8407847503046015E-2</v>
+      </c>
+      <c r="P5" s="10">
         <f t="shared" si="3"/>
+        <v>1.6940770444977552E-2</v>
+      </c>
+      <c r="Q5" s="10">
+        <f>N5/$N$3</f>
         <v>1.0039276286137404</v>
       </c>
-      <c r="N5" s="5">
+      <c r="R5" s="5">
         <f>'Windows (WSL2 - Processus)'!$J$52</f>
         <v>8.4730600000000003</v>
       </c>
-      <c r="O5" s="10">
-        <f>'Windows (WSL2 - Processus)'!$J$54</f>
-        <v>7.0673429285274293E-3</v>
-      </c>
-      <c r="P5" s="10">
+      <c r="S5" s="5">
+        <f>'Windows (WSL2 - Processus)'!$J$53</f>
+        <v>5.9882020673988623E-2</v>
+      </c>
+      <c r="T5" s="10">
         <f t="shared" si="4"/>
+        <v>7.1010165772533961E-3</v>
+      </c>
+      <c r="U5" s="10">
+        <f>R5/$R$3</f>
         <v>1.0047646830027226</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="V5" s="5">
         <f>'Windows (WSL2 - Processus)'!$L$52</f>
         <v>46.33723999999998</v>
       </c>
-      <c r="R5" s="10">
-        <f>'Windows (WSL2 - Processus)'!$L$54</f>
-        <v>4.6198695226596607E-3</v>
-      </c>
-      <c r="S5" s="10">
+      <c r="W5" s="5">
+        <f>'Windows (WSL2 - Processus)'!$L$53</f>
+        <v>0.21407200284016603</v>
+      </c>
+      <c r="X5" s="10">
         <f t="shared" si="5"/>
+        <v>4.6392807727951768E-3</v>
+      </c>
+      <c r="Y5" s="10">
+        <f t="shared" si="6"/>
         <v>1.0042016879568367</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -4159,76 +5439,100 @@
         <f>'Windows (HyperV)'!$B$52</f>
         <v>6.2700000000000006E-2</v>
       </c>
-      <c r="C6" s="10">
-        <f>'Windows (HyperV)'!$B$54</f>
-        <v>3.6543665828993981E-2</v>
+      <c r="C6" s="5">
+        <f>'Windows (HyperV)'!$B$53</f>
+        <v>2.2912878474779228E-3</v>
       </c>
       <c r="D6" s="10">
         <f t="shared" si="0"/>
+        <v>3.764850225892085E-2</v>
+      </c>
+      <c r="E6" s="10">
+        <f>B6/$B$3</f>
         <v>1.0302333223792313</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <f>'Windows (HyperV)'!$D$52</f>
         <v>0.33964</v>
       </c>
-      <c r="F6" s="10">
-        <f>'Windows (HyperV)'!$D$54</f>
-        <v>1.7535340799326442E-2</v>
-      </c>
-      <c r="G6" s="10">
+      <c r="G6" s="5">
+        <f>'Windows (HyperV)'!$D$53</f>
+        <v>5.9557031490832324E-3</v>
+      </c>
+      <c r="H6" s="10">
         <f t="shared" si="1"/>
+        <v>1.7905427061160578E-2</v>
+      </c>
+      <c r="I6" s="10">
+        <f>F6/$F$3</f>
         <v>1.0211051650532137</v>
       </c>
-      <c r="H6" s="5">
+      <c r="J6" s="5">
         <f>'Windows (HyperV)'!$F$52</f>
         <v>0.71206000000000014</v>
       </c>
-      <c r="I6" s="10">
-        <f>'Windows (HyperV)'!$F$54</f>
-        <v>7.1190091655060194E-3</v>
-      </c>
-      <c r="J6" s="10">
+      <c r="K6" s="5">
+        <f>'Windows (HyperV)'!$F$53</f>
+        <v>5.0691616663902173E-3</v>
+      </c>
+      <c r="L6" s="10">
         <f t="shared" si="2"/>
+        <v>7.2468358347251138E-3</v>
+      </c>
+      <c r="M6" s="10">
+        <f>J6/$J$3</f>
         <v>1.0179556826304506</v>
       </c>
-      <c r="K6" s="5">
+      <c r="N6" s="5">
         <f>'Windows (HyperV)'!$H$52</f>
         <v>4.1122800000000002</v>
       </c>
-      <c r="L6" s="10">
-        <f>'Windows (HyperV)'!$H$54</f>
-        <v>1.8325200265252344E-2</v>
-      </c>
-      <c r="M6" s="10">
+      <c r="O6" s="5">
+        <f>'Windows (HyperV)'!$H$53</f>
+        <v>7.535835454679192E-2</v>
+      </c>
+      <c r="P6" s="10">
         <f t="shared" si="3"/>
+        <v>1.8662019520956093E-2</v>
+      </c>
+      <c r="Q6" s="10">
+        <f>N6/$N$3</f>
         <v>1.0183801132226866</v>
       </c>
-      <c r="N6" s="5">
+      <c r="R6" s="5">
         <f>'Windows (HyperV)'!$J$52</f>
         <v>8.6216000000000044</v>
       </c>
-      <c r="O6" s="10">
-        <f>'Windows (HyperV)'!$J$54</f>
-        <v>8.7723554060881882E-3</v>
-      </c>
-      <c r="P6" s="10">
+      <c r="S6" s="5">
+        <f>'Windows (HyperV)'!$J$53</f>
+        <v>7.5631739369129966E-2</v>
+      </c>
+      <c r="T6" s="10">
         <f t="shared" si="4"/>
+        <v>8.9686725494884257E-3</v>
+      </c>
+      <c r="U6" s="10">
+        <f>R6/$R$3</f>
         <v>1.0223790685981544</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="V6" s="5">
         <f>'Windows (HyperV)'!$L$52</f>
         <v>47.437419999999982</v>
       </c>
-      <c r="R6" s="10">
-        <f>'Windows (HyperV)'!$L$54</f>
-        <v>4.051776773270825E-3</v>
-      </c>
-      <c r="S6" s="10">
+      <c r="W6" s="5">
+        <f>'Windows (HyperV)'!$L$53</f>
+        <v>0.19220583653989284</v>
+      </c>
+      <c r="X6" s="10">
         <f t="shared" si="5"/>
+        <v>4.1654061719799528E-3</v>
+      </c>
+      <c r="Y6" s="10">
+        <f t="shared" si="6"/>
         <v>1.0280443383403373</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -4236,76 +5540,100 @@
         <f>'Windows (HyperV - Processus)'!$B$52</f>
         <v>6.1000000000000006E-2</v>
       </c>
-      <c r="C7" s="10">
-        <f>'Windows (HyperV - Processus)'!$B$54</f>
-        <v>4.0422386904714627E-2</v>
+      <c r="C7" s="5">
+        <f>'Windows (HyperV - Processus)'!$B$53</f>
+        <v>2.4657656011875923E-3</v>
       </c>
       <c r="D7" s="10">
         <f t="shared" si="0"/>
+        <v>4.0515373006697213E-2</v>
+      </c>
+      <c r="E7" s="10">
+        <f>B7/$B$3</f>
         <v>1.0023003614853765</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <f>'Windows (HyperV - Processus)'!$D$52</f>
         <v>0.33318000000000003</v>
       </c>
-      <c r="F7" s="10">
-        <f>'Windows (HyperV - Processus)'!$D$54</f>
-        <v>7.9338702582066305E-3</v>
-      </c>
-      <c r="G7" s="10">
+      <c r="G7" s="5">
+        <f>'Windows (HyperV - Processus)'!$D$53</f>
+        <v>2.6434068926292856E-3</v>
+      </c>
+      <c r="H7" s="10">
         <f t="shared" si="1"/>
+        <v>7.947227745262719E-3</v>
+      </c>
+      <c r="I7" s="10">
+        <f>F7/$F$3</f>
         <v>1.0016836029102278</v>
       </c>
-      <c r="H7" s="5">
+      <c r="J7" s="5">
         <f>'Windows (HyperV - Processus)'!$F$52</f>
         <v>0.69896000000000014</v>
       </c>
-      <c r="I7" s="10">
-        <f>'Windows (HyperV - Processus)'!$F$54</f>
-        <v>5.9401327983209552E-3</v>
-      </c>
-      <c r="J7" s="10">
+      <c r="K7" s="5">
+        <f>'Windows (HyperV - Processus)'!$F$53</f>
+        <v>4.1519152207144154E-3</v>
+      </c>
+      <c r="L7" s="10">
         <f t="shared" si="2"/>
+        <v>5.9355471346882278E-3</v>
+      </c>
+      <c r="M7" s="10">
+        <f>J7/$J$3</f>
         <v>0.99922802001429611</v>
       </c>
-      <c r="K7" s="5">
+      <c r="N7" s="5">
         <f>'Windows (HyperV - Processus)'!$H$52</f>
         <v>4.0559399999999997</v>
       </c>
-      <c r="L7" s="10">
-        <f>'Windows (HyperV - Processus)'!$H$54</f>
-        <v>1.6336363900456657E-2</v>
-      </c>
-      <c r="M7" s="10">
+      <c r="O7" s="5">
+        <f>'Windows (HyperV - Processus)'!$H$53</f>
+        <v>6.6259311798418166E-2</v>
+      </c>
+      <c r="P7" s="10">
         <f t="shared" si="3"/>
+        <v>1.6408699176936003E-2</v>
+      </c>
+      <c r="Q7" s="10">
+        <f>N7/$N$3</f>
         <v>1.004427868828101</v>
       </c>
-      <c r="N7" s="5">
+      <c r="R7" s="5">
         <f>'Windows (HyperV - Processus)'!$J$52</f>
         <v>8.4887200000000025</v>
       </c>
-      <c r="O7" s="10">
-        <f>'Windows (HyperV - Processus)'!$J$54</f>
-        <v>4.0208104174399217E-3</v>
-      </c>
-      <c r="P7" s="10">
+      <c r="S7" s="5">
+        <f>'Windows (HyperV - Processus)'!$J$53</f>
+        <v>3.4131533806730625E-2</v>
+      </c>
+      <c r="T7" s="10">
         <f t="shared" si="4"/>
+        <v>4.0474350170677893E-3</v>
+      </c>
+      <c r="U7" s="10">
+        <f>R7/$R$3</f>
         <v>1.0066216998225994</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="V7" s="5">
         <f>'Windows (HyperV - Processus)'!$L$52</f>
         <v>46.445279999999983</v>
       </c>
-      <c r="R7" s="10">
-        <f>'Windows (HyperV - Processus)'!$L$54</f>
-        <v>3.7398917875664985E-3</v>
-      </c>
-      <c r="S7" s="10">
+      <c r="W7" s="5">
+        <f>'Windows (HyperV - Processus)'!$L$53</f>
+        <v>0.17370032124322649</v>
+      </c>
+      <c r="X7" s="10">
         <f t="shared" si="5"/>
+        <v>3.7643622233670565E-3</v>
+      </c>
+      <c r="Y7" s="10">
+        <f t="shared" si="6"/>
         <v>1.0065430865892728</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
@@ -4313,76 +5641,100 @@
         <f>'Linux (Natif)'!$B$52</f>
         <v>6.2859999999999999E-2</v>
       </c>
-      <c r="C8" s="10">
-        <f>'Linux (Natif)'!$B$54</f>
+      <c r="C8" s="5">
+        <f>'Linux (Natif)'!$B$53</f>
+        <v>2.6382570003697526E-3</v>
+      </c>
+      <c r="D8" s="10">
+        <f>C8/$B$8</f>
         <v>4.1970362716668035E-2</v>
       </c>
-      <c r="D8" s="10">
+      <c r="E8" s="10">
         <f>B8/$B$8</f>
         <v>1</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <f>'Linux (Natif)'!$D$52</f>
         <v>0.33532000000000006</v>
       </c>
-      <c r="F8" s="10">
-        <f>'Linux (Natif)'!$D$54</f>
+      <c r="G8" s="5">
+        <f>'Linux (Natif)'!$D$53</f>
+        <v>3.7600000000000008E-3</v>
+      </c>
+      <c r="H8" s="10">
+        <f>G8/$F$8</f>
         <v>1.1213169509722056E-2</v>
       </c>
-      <c r="G8" s="10">
-        <f>E8/$E$8</f>
+      <c r="I8" s="10">
+        <f>F8/$F$8</f>
         <v>1</v>
       </c>
-      <c r="H8" s="5">
+      <c r="J8" s="5">
         <f>'Linux (Natif)'!$F$52</f>
         <v>0.70478000000000018</v>
       </c>
-      <c r="I8" s="10">
-        <f>'Linux (Natif)'!$F$54</f>
+      <c r="K8" s="5">
+        <f>'Linux (Natif)'!$F$53</f>
+        <v>5.2126384873689511E-3</v>
+      </c>
+      <c r="L8" s="10">
+        <f>K8/$J$8</f>
         <v>7.3961214667966598E-3</v>
       </c>
-      <c r="J8" s="10">
-        <f>H8/$H$8</f>
+      <c r="M8" s="10">
+        <f>J8/$J$8</f>
         <v>1</v>
       </c>
-      <c r="K8" s="5">
+      <c r="N8" s="5">
         <f>'Linux (Natif)'!$H$52</f>
         <v>4.0511999999999997</v>
       </c>
-      <c r="L8" s="10">
-        <f>'Linux (Natif)'!$H$54</f>
+      <c r="O8" s="5">
+        <f>'Linux (Natif)'!$H$53</f>
+        <v>7.7899679075077083E-2</v>
+      </c>
+      <c r="P8" s="10">
+        <f>O8/$N$8</f>
         <v>1.9228791240885931E-2</v>
       </c>
-      <c r="M8" s="10">
-        <f>K8/$K$8</f>
+      <c r="Q8" s="10">
+        <f>N8/$N$8</f>
         <v>1</v>
       </c>
-      <c r="N8" s="5">
+      <c r="R8" s="5">
         <f>'Linux (Natif)'!$J$52</f>
         <v>8.4575399999999998</v>
       </c>
-      <c r="O8" s="10">
-        <f>'Linux (Natif)'!$J$54</f>
+      <c r="S8" s="5">
+        <f>'Linux (Natif)'!$J$53</f>
+        <v>7.7605466302316586E-2</v>
+      </c>
+      <c r="T8" s="10">
+        <f>S8/$R$8</f>
         <v>9.1758911341024204E-3</v>
       </c>
-      <c r="P8" s="10">
-        <f>N8/$N$8</f>
+      <c r="U8" s="10">
+        <f>R8/$R$8</f>
         <v>1</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="V8" s="5">
         <f>'Linux (Natif)'!$L$52</f>
         <v>46.305420000000005</v>
       </c>
-      <c r="R8" s="10">
-        <f>'Linux (Natif)'!$L$54</f>
+      <c r="W8" s="5">
+        <f>'Linux (Natif)'!$L$53</f>
+        <v>0.15479923643222562</v>
+      </c>
+      <c r="X8" s="10">
+        <f>W8/$V$8</f>
         <v>3.343004694314955E-3</v>
       </c>
-      <c r="S8" s="10">
-        <f>Q8/$Q$8</f>
+      <c r="Y8" s="10">
+        <f>V8/$V$8</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
@@ -4390,72 +5742,96 @@
         <f>'Linux (Docker)'!$B$52</f>
         <v>6.5179999999999988E-2</v>
       </c>
-      <c r="C9" s="10">
-        <f>'Linux (Docker)'!$B$54</f>
-        <v>5.1954349534846435E-2</v>
+      <c r="C9" s="5">
+        <f>'Linux (Docker)'!$B$53</f>
+        <v>3.3863845026812899E-3</v>
       </c>
       <c r="D9" s="10">
+        <f>C9/$B$8</f>
+        <v>5.387185018583026E-2</v>
+      </c>
+      <c r="E9" s="10">
         <f>B9/$B$8</f>
         <v>1.0369074132993954</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <f>'Linux (Docker)'!$D$52</f>
         <v>0.34699999999999998</v>
       </c>
-      <c r="F9" s="10">
-        <f>'Linux (Docker)'!$D$54</f>
-        <v>1.9194035510486093E-2</v>
-      </c>
-      <c r="G9" s="10">
-        <f>E9/$E$8</f>
+      <c r="G9" s="5">
+        <f>'Linux (Docker)'!$D$53</f>
+        <v>6.6603303221386733E-3</v>
+      </c>
+      <c r="H9" s="10">
+        <f>G9/$F$8</f>
+        <v>1.9862609811936872E-2</v>
+      </c>
+      <c r="I9" s="10">
+        <f>F9/$F$8</f>
         <v>1.0348323989025405</v>
       </c>
-      <c r="H9" s="5">
+      <c r="J9" s="5">
         <f>'Linux (Docker)'!$F$52</f>
         <v>0.73458000000000023</v>
       </c>
-      <c r="I9" s="10">
-        <f>'Linux (Docker)'!$F$54</f>
-        <v>1.1367129336496614E-2</v>
-      </c>
-      <c r="J9" s="10">
-        <f>H9/$H$8</f>
+      <c r="K9" s="5">
+        <f>'Linux (Docker)'!$F$53</f>
+        <v>8.3500658680036848E-3</v>
+      </c>
+      <c r="L9" s="10">
+        <f>K9/$J$8</f>
+        <v>1.1847762235028921E-2</v>
+      </c>
+      <c r="M9" s="10">
+        <f>J9/$J$8</f>
         <v>1.0422826981469395</v>
       </c>
-      <c r="K9" s="5">
+      <c r="N9" s="5">
         <f>'Linux (Docker)'!$H$52</f>
         <v>4.2602200000000003</v>
       </c>
-      <c r="L9" s="10">
-        <f>'Linux (Docker)'!$H$54</f>
-        <v>1.5961084712791708E-2</v>
-      </c>
-      <c r="M9" s="10">
-        <f>K9/$K$8</f>
+      <c r="O9" s="5">
+        <f>'Linux (Docker)'!$H$53</f>
+        <v>6.7997732315129497E-2</v>
+      </c>
+      <c r="P9" s="10">
+        <f>O9/$N$8</f>
+        <v>1.6784590322652424E-2</v>
+      </c>
+      <c r="Q9" s="10">
+        <f>N9/$N$8</f>
         <v>1.051594589257504</v>
       </c>
-      <c r="N9" s="5">
+      <c r="R9" s="5">
         <f>'Linux (Docker)'!$J$52</f>
         <v>8.941119999999998</v>
       </c>
-      <c r="O9" s="10">
-        <f>'Linux (Docker)'!$J$54</f>
-        <v>8.937819187904714E-3</v>
-      </c>
-      <c r="P9" s="10">
-        <f>N9/$N$8</f>
+      <c r="S9" s="5">
+        <f>'Linux (Docker)'!$J$53</f>
+        <v>7.9914113897358585E-2</v>
+      </c>
+      <c r="T9" s="10">
+        <f>S9/$R$8</f>
+        <v>9.4488602947616664E-3</v>
+      </c>
+      <c r="U9" s="10">
+        <f>R9/$R$8</f>
         <v>1.0571773825485895</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="V9" s="5">
         <f>'Linux (Docker)'!$L$52</f>
         <v>49.848280000000003</v>
       </c>
-      <c r="R9" s="10">
-        <f>'Linux (Docker)'!$L$54</f>
-        <v>3.5648143489678498E-3</v>
-      </c>
-      <c r="S9" s="10">
-        <f>Q9/$Q$8</f>
+      <c r="W9" s="5">
+        <f>'Linux (Docker)'!$L$53</f>
+        <v>0.17769986381536709</v>
+      </c>
+      <c r="X9" s="10">
+        <f>W9/$V$8</f>
+        <v>3.8375607826333737E-3</v>
+      </c>
+      <c r="Y9" s="10">
+        <f>V9/$V$8</f>
         <v>1.0765106978837466</v>
       </c>
     </row>
@@ -6156,7 +7532,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D53633E4-B3A2-4836-8621-294DFDF88276}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{263FB86D-35E9-4665-BD76-C9655B1CD1C7}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -6167,8 +7543,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (Natif)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (Natif)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{A013061F-6225-4DD5-BD9A-18CCAA165F09}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (Natif)'!J2:J51</xm:f>
+              <xm:sqref>J55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0AC99F70-1986-4530-85CD-87DAB941F78A}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (Natif)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D6051AD8-E20E-4C7E-83A6-FB1D6D67759B}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (Natif)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -6188,7 +7612,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D6051AD8-E20E-4C7E-83A6-FB1D6D67759B}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{D53633E4-B3A2-4836-8621-294DFDF88276}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -6199,56 +7623,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (Natif)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0AC99F70-1986-4530-85CD-87DAB941F78A}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (Natif)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{A013061F-6225-4DD5-BD9A-18CCAA165F09}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (Natif)'!J2:J51</xm:f>
-              <xm:sqref>J55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{263FB86D-35E9-4665-BD76-C9655B1CD1C7}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (Natif)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (Natif)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -6262,8 +7638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED430D83-B77A-4463-B87E-697C6F0E186E}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L55" sqref="L55"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7642,7 +9018,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0FA95288-A489-4585-94C4-768758F6474C}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{26BC4944-7654-4BFA-9F72-24B1C359120F}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -7653,8 +9029,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (WSL2)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{9A042822-AA4C-4325-91C6-EC1952126EF5}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2)'!J2:J51</xm:f>
+              <xm:sqref>J55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0FA84A2C-672E-44AC-ACAA-ED61E0BF21BE}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{BBA6465A-E308-4DD6-9A70-F5CB35F82A61}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -7674,7 +9098,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{BBA6465A-E308-4DD6-9A70-F5CB35F82A61}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0FA95288-A489-4585-94C4-768758F6474C}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -7685,56 +9109,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0FA84A2C-672E-44AC-ACAA-ED61E0BF21BE}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{9A042822-AA4C-4325-91C6-EC1952126EF5}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!J2:J51</xm:f>
-              <xm:sqref>J55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{26BC4944-7654-4BFA-9F72-24B1C359120F}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (WSL2)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -9127,7 +10503,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DFB037B2-CCDD-4B71-9593-4095BEADE567}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{CFB2627E-8967-4A81-83E6-676B520A3425}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -9138,8 +10514,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (WSL2 - Processus)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0E15ECCC-D6F8-4C4D-92AF-59C6E4AAB5F5}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2 - Processus)'!J2:J51</xm:f>
+              <xm:sqref>J55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{6B49AE29-6C9E-480F-8A0D-77BC2859D87C}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2 - Processus)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{98184E74-9215-4257-A184-37176536AAA8}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (WSL2 - Processus)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -9159,7 +10583,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{98184E74-9215-4257-A184-37176536AAA8}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DFB037B2-CCDD-4B71-9593-4095BEADE567}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -9170,56 +10594,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{6B49AE29-6C9E-480F-8A0D-77BC2859D87C}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0E15ECCC-D6F8-4C4D-92AF-59C6E4AAB5F5}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!J2:J51</xm:f>
-              <xm:sqref>J55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{CFB2627E-8967-4A81-83E6-676B520A3425}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (WSL2 - Processus)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (WSL2 - Processus)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -10612,7 +11988,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{CB50B3B6-4016-48CB-8198-CE38282339F8}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5DC8D8CB-A05A-4FE8-BCF8-8A2476066B3F}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -10623,8 +11999,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (HyperV)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{49825F7F-A3D8-485F-87F3-FA080CBEF77E}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV)'!J2:J51</xm:f>
+              <xm:sqref>J55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{948B6A77-9CAD-4F96-B620-E4761B6E212C}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DDFF044F-6546-4CF0-963C-9764D1216A74}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -10644,7 +12068,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DDFF044F-6546-4CF0-963C-9764D1216A74}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{CB50B3B6-4016-48CB-8198-CE38282339F8}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -10655,56 +12079,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{948B6A77-9CAD-4F96-B620-E4761B6E212C}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{49825F7F-A3D8-485F-87F3-FA080CBEF77E}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!J2:J51</xm:f>
-              <xm:sqref>J55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5DC8D8CB-A05A-4FE8-BCF8-8A2476066B3F}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (HyperV)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -12097,7 +13473,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{3B759F57-5925-482A-9086-0B51A14E2420}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0B58E305-8FE4-447D-AD29-B0D933ADB202}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -12108,8 +13484,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Windows (HyperV - Processus)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{64D832F5-81D9-4F2C-A67B-1F115BAA9FD7}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV - Processus)'!J2:J51</xm:f>
+              <xm:sqref>J55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{48A1F807-54EC-4B10-844B-207851B03EB3}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV - Processus)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B4EACD82-77AA-48D9-A91E-A39ABF91BBAB}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Windows (HyperV - Processus)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -12129,7 +13553,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B4EACD82-77AA-48D9-A91E-A39ABF91BBAB}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{3B759F57-5925-482A-9086-0B51A14E2420}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -12140,56 +13564,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{48A1F807-54EC-4B10-844B-207851B03EB3}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{64D832F5-81D9-4F2C-A67B-1F115BAA9FD7}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!J2:J51</xm:f>
-              <xm:sqref>J55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{0B58E305-8FE4-447D-AD29-B0D933ADB202}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Windows (HyperV - Processus)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Windows (HyperV - Processus)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -13582,7 +14958,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{05DF6556-8BB2-4C26-BA82-557146EF9EEF}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{C422E0C4-9C93-4E2A-A077-186C8471DC37}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -13593,8 +14969,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Linux (Natif)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Linux (Natif)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{989BB518-1281-4EE1-A69F-0DA933D1EB28}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Natif)'!J2:J51</xm:f>
+              <xm:sqref>J55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5411D816-8D3B-4A0E-A036-09C6F257009C}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Natif)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{1FA50543-1619-4C76-BA32-FA54FFF9EEF0}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Natif)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -13614,7 +15038,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{1FA50543-1619-4C76-BA32-FA54FFF9EEF0}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{05DF6556-8BB2-4C26-BA82-557146EF9EEF}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -13625,56 +15049,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Linux (Natif)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{5411D816-8D3B-4A0E-A036-09C6F257009C}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Natif)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{989BB518-1281-4EE1-A69F-0DA933D1EB28}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Natif)'!J2:J51</xm:f>
-              <xm:sqref>J55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{C422E0C4-9C93-4E2A-A077-186C8471DC37}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Natif)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Linux (Natif)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -15067,7 +16443,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{8A9F5D4B-DC6F-47C4-90FC-816734A33D56}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{7AF38403-7A79-4F1E-8FAD-23629879CF02}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -15078,8 +16454,56 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Linux (Docker)'!B2:B51</xm:f>
-              <xm:sqref>B55</xm:sqref>
+              <xm:f>'Linux (Docker)'!L2:L51</xm:f>
+              <xm:sqref>L55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{76270A85-4189-4518-B8ED-03320A93117D}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Docker)'!J2:J51</xm:f>
+              <xm:sqref>J55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B0D1C296-46A8-49F3-BBE8-C4AF5BB63750}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Docker)'!H2:H51</xm:f>
+              <xm:sqref>H55</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DCCDEE7B-7404-4AB4-BFE7-57E07920CD05}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Linux (Docker)'!F2:F51</xm:f>
+              <xm:sqref>F55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -15099,7 +16523,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{DCCDEE7B-7404-4AB4-BFE7-57E07920CD05}">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{8A9F5D4B-DC6F-47C4-90FC-816734A33D56}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -15110,56 +16534,8 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Linux (Docker)'!F2:F51</xm:f>
-              <xm:sqref>F55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{B0D1C296-46A8-49F3-BBE8-C4AF5BB63750}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Docker)'!H2:H51</xm:f>
-              <xm:sqref>H55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{76270A85-4189-4518-B8ED-03320A93117D}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Docker)'!J2:J51</xm:f>
-              <xm:sqref>J55</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" xr2:uid="{7AF38403-7A79-4F1E-8FAD-23629879CF02}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Linux (Docker)'!L2:L51</xm:f>
-              <xm:sqref>L55</xm:sqref>
+              <xm:f>'Linux (Docker)'!B2:B51</xm:f>
+              <xm:sqref>B55</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>